<commit_message>
Update player table script and add 2025 data files
</commit_message>
<xml_diff>
--- a/Data/Team Goal Distribution/Goal distribution A Lyga Teams 2025.xlsx
+++ b/Data/Team Goal Distribution/Goal distribution A Lyga Teams 2025.xlsx
@@ -503,63 +503,63 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Hegelmann Litauen</t>
+          <t>Sūduva</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Žalgiris</t>
+          <t>Hegelmann Litauen</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
         <v>2</v>
@@ -568,28 +568,28 @@
         <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K3" t="n">
         <v>2</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Banga</t>
+          <t>Kauno Žalgiris</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -602,10 +602,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
         <v>3</v>
@@ -620,139 +620,139 @@
         <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
         <v>2</v>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Dainava</t>
+          <t>Banga</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>3</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L5" t="n">
         <v>2</v>
       </c>
       <c r="M5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Riteriai</t>
+          <t>Dainava</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
         <v>2</v>
       </c>
       <c r="J6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Džiugas Telšiai</t>
+          <t>Riteriai</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
         <v>1</v>
@@ -761,26 +761,26 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Panevėžys</t>
+          <t>Džiugas Telšiai</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" t="n">
         <v>2</v>
@@ -789,35 +789,35 @@
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
         <v>2</v>
       </c>
       <c r="M8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Kauno Žalgiris</t>
+          <t>Šiauliai</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>2</v>
@@ -826,105 +826,105 @@
         <v>3</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
         <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Sūduva</t>
+          <t>Žalgiris</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Šiauliai</t>
+          <t>Panevėžys</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
         <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11" t="n">
         <v>3</v>

</xml_diff>

<commit_message>
Updated data and functions
</commit_message>
<xml_diff>
--- a/Data/Team Goal Distribution/Goal distribution A Lyga Teams 2025.xlsx
+++ b/Data/Team Goal Distribution/Goal distribution A Lyga Teams 2025.xlsx
@@ -503,155 +503,155 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Sūduva</t>
+          <t>Riteriai</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L2" t="n">
         <v>4</v>
       </c>
       <c r="M2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Hegelmann Litauen</t>
+          <t>Šiauliai</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Kauno Žalgiris</t>
+          <t>Hegelmann Litauen</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Banga</t>
+          <t>Kauno Žalgiris</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -663,271 +663,271 @@
         <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Dainava</t>
+          <t>Džiugas Telšiai</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>5</v>
+      </c>
+      <c r="K6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>3</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" t="n">
-        <v>4</v>
-      </c>
-      <c r="K6" t="n">
-        <v>3</v>
-      </c>
       <c r="L6" t="n">
         <v>3</v>
       </c>
       <c r="M6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Riteriai</t>
+          <t>Banga</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>4</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
         <v>4</v>
       </c>
       <c r="K7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Džiugas Telšiai</t>
+          <t>Sūduva</t>
         </is>
       </c>
       <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" t="n">
         <v>0</v>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3</v>
-      </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Šiauliai</t>
+          <t>Žalgiris</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" t="n">
         <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I9" t="n">
         <v>3</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L9" t="n">
         <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Žalgiris</t>
+          <t>Panevėžys</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Panevėžys</t>
+          <t>Dainava</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K11" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L11" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M11" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>